<commit_message>
added point intersection test
</commit_message>
<xml_diff>
--- a/src/main/resources/intersects-tests.xlsx
+++ b/src/main/resources/intersects-tests.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Intersects Source" sheetId="1" r:id="rId1"/>
     <sheet name="Prepared Intersects Source" sheetId="2" r:id="rId2"/>
     <sheet name="Difference Source" sheetId="3" r:id="rId3"/>
     <sheet name="Charts" sheetId="4" r:id="rId4"/>
+    <sheet name="Point Intersection" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId5"/>
-    <pivotCache cacheId="22" r:id="rId6"/>
-    <pivotCache cacheId="26" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>#Target Vertices</t>
   </si>
@@ -162,13 +163,35 @@
   <si>
     <t>Target:1310720</t>
   </si>
+  <si>
+    <t>#Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #Query Vertices</t>
+  </si>
+  <si>
+    <t>Prepared</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Speed Advantage (Prepared over Regular)</t>
+  </si>
+  <si>
+    <t>Regular - Prepared (msec)</t>
+  </si>
+  <si>
+    <t>Time for 1,000,000 features (minutes)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -677,7 +700,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -694,6 +717,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -739,7 +763,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="31">
     <dxf>
       <border>
         <left style="thin">
@@ -993,275 +1017,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF7030A0"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7030A0"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7030A0"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7030A0"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF7030A0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF7030A0"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="6" tint="0.59999389629810485"/>
@@ -1492,6 +1247,17 @@
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00000"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1549,7 +1315,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2624,11 +2389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354461248"/>
-        <c:axId val="354460072"/>
+        <c:axId val="318086544"/>
+        <c:axId val="318088112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354461248"/>
+        <c:axId val="318086544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,7 +2454,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2749,12 +2513,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354460072"/>
+        <c:crossAx val="318088112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354460072"/>
+        <c:axId val="318088112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2815,7 +2579,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2879,7 +2642,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354461248"/>
+        <c:crossAx val="318086544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2893,7 +2656,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3007,7 +2769,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6374,11 +6135,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354461640"/>
-        <c:axId val="354462816"/>
+        <c:axId val="318088896"/>
+        <c:axId val="372483104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354461640"/>
+        <c:axId val="318088896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6439,7 +6200,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6503,12 +6263,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354462816"/>
+        <c:crossAx val="372483104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354462816"/>
+        <c:axId val="372483104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6574,7 +6334,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6638,7 +6397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354461640"/>
+        <c:crossAx val="318088896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6652,7 +6411,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6766,7 +6524,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10133,11 +9890,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="351266240"/>
-        <c:axId val="351267808"/>
+        <c:axId val="372479184"/>
+        <c:axId val="372478008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="351266240"/>
+        <c:axId val="372479184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10198,7 +9955,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10262,12 +10018,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351267808"/>
+        <c:crossAx val="372478008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="351267808"/>
+        <c:axId val="372478008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10324,6 +10080,789 @@
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>Time improvement (msec) for prepared geometry</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372479184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (minutes) to intersect 1,000,000 points vs. query geometry size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Point Intersection'!$I$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Regular</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Point Intersection'!$H$28:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20480</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81920</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>163840</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>327680</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>655360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1310720</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Point Intersection'!$I$28:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.2951142984973669E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4306923726388001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4167685038254831E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7258721415201666E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9731542256677833E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2967869873047168E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8327504781091497E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0452136637371502E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.670828491211149E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12120460133870467</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22961507700602335</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45295555816649669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.88884315043130002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7809635539754001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5585293596393663</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1245724971516493</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.217249176940816</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.31617895131367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Point Intersection'!$J$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prepared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Point Intersection'!$H$28:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20480</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81920</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>163840</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>327680</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>655360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1310720</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Point Intersection'!$J$28:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.0007836710611584E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4205580647788999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7463421630866168E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7728173828150834E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0240307617188837E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.276568094889317E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9491241455078E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0606663004560494E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2440167236322168E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5405482991546833E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9598132324204999E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5707285563150999E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5486284383159337E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7376308186838339E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.9809720865896506E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0229964192748329E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3161315612785083E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.1187196756982333E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="517748680"/>
+        <c:axId val="517748288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="517748680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># Vertices in query geometry</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="517748288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="517748288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (minutes)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10392,7 +10931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351266240"/>
+        <c:crossAx val="517748680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10472,7 +11011,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -10557,6 +11095,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12210,6 +12788,544 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -12578,6 +13694,41 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="bennight" refreshedDate="42169.843780555559" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="324">
   <cacheSource type="worksheet">
@@ -17967,7 +19118,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="G4:Y23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0">
@@ -18141,7 +19292,7 @@
     <format dxfId="30">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="29">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -18150,7 +19301,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="28">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18164,7 +19315,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="G4:Y23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0">
@@ -18336,13 +19487,13 @@
     <dataField name="Sum of MSEC" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="54">
+    <format dxfId="27">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="25">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18356,7 +19507,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="G4:Y23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0">
@@ -18527,7 +19678,7 @@
     <dataField name="Sum of Regular - Prepared" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="24">
-    <format dxfId="50">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18546,7 +19697,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18558,7 +19709,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18571,7 +19722,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18584,7 +19735,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18596,7 +19747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18608,7 +19759,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18620,7 +19771,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18632,7 +19783,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18644,7 +19795,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -18663,14 +19814,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -18834,7 +19985,7 @@
     </format>
   </formats>
   <conditionalFormats count="2">
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -18845,7 +19996,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -30456,7 +31607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y23" sqref="G4:Y23"/>
     </sheetView>
   </sheetViews>
@@ -38412,7 +39563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="H6:Y23">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38433,4 +39584,1051 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C5" s="2">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12">
+        <v>6.0047020263669505E-4</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.103521912752622</v>
+      </c>
+      <c r="H5" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4.3770685790984198E-3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.50851632063985597</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2.0523348388673399E-4</v>
+      </c>
+      <c r="E6" s="12">
+        <v>3.30220576194448E-4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I6" s="2">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.0584154235832801E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.2895485074657503E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C7" s="2">
+        <v>40</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1.64780529785197E-4</v>
+      </c>
+      <c r="E7" s="12">
+        <v>4.5190515674701798E-4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I7" s="2">
+        <v>40</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.45006110229529E-3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4.3938642382586199E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C8" s="2">
+        <v>80</v>
+      </c>
+      <c r="D8" s="12">
+        <v>2.2636904296890499E-4</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4.26601291548694E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I8" s="2">
+        <v>80</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.0355232849121E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2.2663483749800501E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C9" s="2">
+        <v>160</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1.21441845703133E-4</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5.1740402591217102E-4</v>
+      </c>
+      <c r="H9" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I9" s="2">
+        <v>160</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.18389253540067E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>3.9164907202745201E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C10" s="2">
+        <v>320</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1.3659408569335901E-4</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1.31648887755637E-3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I10" s="2">
+        <v>320</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.3780721923828301E-3</v>
+      </c>
+      <c r="K10" s="2">
+        <v>6.9139043383726999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C11" s="2">
+        <v>640</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.16947448730468E-4</v>
+      </c>
+      <c r="E11" s="12">
+        <v>9.8809849727546795E-4</v>
+      </c>
+      <c r="H11" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I11" s="2">
+        <v>640</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.6996502868654899E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4.6692384793465699E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1280</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1.2363997802736299E-4</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1.7332343776703201E-3</v>
+      </c>
+      <c r="H12" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1280</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2.42712819824229E-3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>3.7659932080770002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2560</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1.34641003417933E-4</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3.3390308847146199E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2560</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4.0024970947266899E-3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3.8807465926804702E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5120</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1.5243289794928099E-4</v>
+      </c>
+      <c r="E14" s="12">
+        <v>5.9552707028929803E-3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5120</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.2722760803222803E-3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>4.0535615174607298E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C15" s="2">
+        <v>10240</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1.7758879394522999E-4</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1.0321287219409701E-2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10240</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.3776904620361401E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>8.1896566048237404E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C16" s="2">
+        <v>20480</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2.14243713378906E-4</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1.8519964893039999E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I16" s="2">
+        <v>20480</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2.71773334899898E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.113222848700819</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C17" s="2">
+        <v>40960</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2.12917706298956E-4</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1.6040361643771602E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I17" s="2">
+        <v>40960</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5.3330589025877999E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.144819776381377</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C18" s="2">
+        <v>81920</v>
+      </c>
+      <c r="D18" s="12">
+        <v>2.8425784912103E-4</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1.6907353478828099E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I18" s="2">
+        <v>81920</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.106857813238524</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.26218200294759503</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C19" s="2">
+        <v>163840</v>
+      </c>
+      <c r="D19" s="12">
+        <v>3.5885832519537902E-4</v>
+      </c>
+      <c r="E19" s="12">
+        <v>2.02874449497518E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I19" s="2">
+        <v>163840</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.21351176157836199</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.52137631197995604</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C20" s="2">
+        <v>327680</v>
+      </c>
+      <c r="D20" s="12">
+        <v>4.8137978515649E-4</v>
+      </c>
+      <c r="E20" s="12">
+        <v>3.4569765465460103E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I20" s="2">
+        <v>327680</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.42747434982909899</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.96753097695586798</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C21" s="2">
+        <v>655360</v>
+      </c>
+      <c r="D21" s="12">
+        <v>7.8967893676710501E-4</v>
+      </c>
+      <c r="E21" s="12">
+        <v>6.7871616523716302E-2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I21" s="2">
+        <v>655360</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.85303495061644896</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.904314036917</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>163840</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1310720</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1.2712318054189399E-3</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0.13793980184926999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>163840</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1310720</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.6989707370788201</v>
+      </c>
+      <c r="K22" s="2">
+        <v>4.0481000373609097</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f>B4</f>
+        <v>#Points</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" ref="C27:C48" si="0">C4</f>
+        <v xml:space="preserve"> #Query Vertices</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" t="str">
+        <f>C27</f>
+        <v xml:space="preserve"> #Query Vertices</v>
+      </c>
+      <c r="I27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <f t="shared" ref="B28:C28" si="1">B5</f>
+        <v>163840</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D28" s="12">
+        <f>J5-D5</f>
+        <v>3.7765983764617246E-3</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" ref="H28:H45" si="2">C28</f>
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <f>J5 / 1000 / 60 * 1000000</f>
+        <v>7.2951142984973669E-2</v>
+      </c>
+      <c r="J28">
+        <f>D5/1000/60*1000000</f>
+        <v>1.0007836710611584E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <f t="shared" ref="B29:C29" si="3">B6</f>
+        <v>163840</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D29" s="12">
+        <f t="shared" ref="D29:D45" si="4">J6-D6</f>
+        <v>1.853181939696546E-3</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="H29" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" ref="I29:I45" si="5">J6 / 1000 / 60 * 1000000</f>
+        <v>3.4306923726388001E-2</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" ref="J29:J45" si="6">D6/1000/60*1000000</f>
+        <v>3.4205580647788999E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <f t="shared" ref="B30:C30" si="7">B7</f>
+        <v>163840</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D30" s="12">
+        <f t="shared" si="4"/>
+        <v>1.2852805725100929E-3</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="H30" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="5"/>
+        <v>2.4167685038254831E-2</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="6"/>
+        <v>2.7463421630866168E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <f t="shared" ref="B31:C31" si="8">B8</f>
+        <v>163840</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="D31" s="12">
+        <f t="shared" si="4"/>
+        <v>8.0915424194319494E-4</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="H31" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="5"/>
+        <v>1.7258721415201666E-2</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="6"/>
+        <v>3.7728173828150834E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <f t="shared" ref="B32:C32" si="9">B9</f>
+        <v>163840</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="D32" s="12">
+        <f t="shared" si="4"/>
+        <v>1.0624506896975369E-3</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="H32" s="2">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9731542256677833E-2</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="6"/>
+        <v>2.0240307617188837E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <f t="shared" ref="B33:C33" si="10">B10</f>
+        <v>163840</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="D33" s="12">
+        <f t="shared" si="4"/>
+        <v>1.2414781066894711E-3</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="H33" s="2">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="5"/>
+        <v>2.2967869873047168E-2</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="6"/>
+        <v>2.276568094889317E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <f t="shared" ref="B34:C34" si="11">B11</f>
+        <v>163840</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+      <c r="D34" s="12">
+        <f t="shared" si="4"/>
+        <v>1.582702838135022E-3</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="H34" s="2">
+        <f t="shared" si="2"/>
+        <v>640</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="5"/>
+        <v>2.8327504781091497E-2</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9491241455078E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <f t="shared" ref="B35:C35" si="12">B12</f>
+        <v>163840</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+      <c r="D35" s="12">
+        <f t="shared" si="4"/>
+        <v>2.3034882202149268E-3</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="H35" s="2">
+        <f t="shared" si="2"/>
+        <v>1280</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="5"/>
+        <v>4.0452136637371502E-2</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="6"/>
+        <v>2.0606663004560494E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <f t="shared" ref="B36:C36" si="13">B13</f>
+        <v>163840</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+      <c r="D36" s="12">
+        <f t="shared" si="4"/>
+        <v>3.8678560913087568E-3</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="H36" s="2">
+        <f t="shared" si="2"/>
+        <v>2560</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="5"/>
+        <v>6.670828491211149E-2</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="6"/>
+        <v>2.2440167236322168E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <f t="shared" ref="B37:C37" si="14">B14</f>
+        <v>163840</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>5120</v>
+      </c>
+      <c r="D37" s="12">
+        <f t="shared" si="4"/>
+        <v>7.1198431823729993E-3</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
+        <v>5120</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="5"/>
+        <v>0.12120460133870467</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="6"/>
+        <v>2.5405482991546833E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <f t="shared" ref="B38:C38" si="15">B15</f>
+        <v>163840</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>10240</v>
+      </c>
+      <c r="D38" s="12">
+        <f t="shared" si="4"/>
+        <v>1.3599315826416171E-2</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="H38" s="2">
+        <f t="shared" si="2"/>
+        <v>10240</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="5"/>
+        <v>0.22961507700602335</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9598132324204999E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <f t="shared" ref="B39:C39" si="16">B16</f>
+        <v>163840</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>20480</v>
+      </c>
+      <c r="D39" s="12">
+        <f t="shared" si="4"/>
+        <v>2.6963089776610893E-2</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="H39" s="2">
+        <f t="shared" si="2"/>
+        <v>20480</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="5"/>
+        <v>0.45295555816649669</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5707285563150999E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <f t="shared" ref="B40:C40" si="17">B17</f>
+        <v>163840</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>40960</v>
+      </c>
+      <c r="D40" s="12">
+        <f t="shared" si="4"/>
+        <v>5.3117671319579042E-2</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="H40" s="2">
+        <f t="shared" si="2"/>
+        <v>40960</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="5"/>
+        <v>0.88884315043130002</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5486284383159337E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <f t="shared" ref="B41:C41" si="18">B18</f>
+        <v>163840</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>81920</v>
+      </c>
+      <c r="D41" s="12">
+        <f t="shared" si="4"/>
+        <v>0.10657355538940297</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="H41" s="2">
+        <f t="shared" si="2"/>
+        <v>81920</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="5"/>
+        <v>1.7809635539754001</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="6"/>
+        <v>4.7376308186838339E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <f t="shared" ref="B42:C42" si="19">B19</f>
+        <v>163840</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>163840</v>
+      </c>
+      <c r="D42" s="12">
+        <f t="shared" si="4"/>
+        <v>0.2131529032531666</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="H42" s="2">
+        <f t="shared" si="2"/>
+        <v>163840</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="5"/>
+        <v>3.5585293596393663</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="6"/>
+        <v>5.9809720865896506E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <f t="shared" ref="B43:C43" si="20">B20</f>
+        <v>163840</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>327680</v>
+      </c>
+      <c r="D43" s="12">
+        <f t="shared" si="4"/>
+        <v>0.42699297004394249</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="H43" s="2">
+        <f t="shared" si="2"/>
+        <v>327680</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="5"/>
+        <v>7.1245724971516493</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="6"/>
+        <v>8.0229964192748329E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <f t="shared" ref="B44:C44" si="21">B21</f>
+        <v>163840</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>655360</v>
+      </c>
+      <c r="D44" s="12">
+        <f t="shared" si="4"/>
+        <v>0.85224527167968189</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="H44" s="2">
+        <f t="shared" si="2"/>
+        <v>655360</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="5"/>
+        <v>14.217249176940816</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3161315612785083E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <f t="shared" ref="B45:C45" si="22">B22</f>
+        <v>163840</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>1310720</v>
+      </c>
+      <c r="D45" s="12">
+        <f t="shared" si="4"/>
+        <v>1.6976995052734012</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="H45" s="2">
+        <f t="shared" si="2"/>
+        <v>1310720</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="5"/>
+        <v>28.31617895131367</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1187196756982333E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>